<commit_message>
refactor: terminar de tratar ABRIL 2023
</commit_message>
<xml_diff>
--- a/Base de Dados/Dados Tratados/ABRIL_2023.xlsx
+++ b/Base de Dados/Dados Tratados/ABRIL_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GitHub\Projeto-Painel-de-BI-Dados-Agricolas\Base de Dados\Dados Tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732C21F-1D4F-4034-857A-5BC584792D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0D2584-B1C4-4F2F-84A8-5855C2D4AA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AREA_POR_PRODUTO" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,16 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -485,6 +494,18 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -516,6 +537,141 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -626,76 +782,10 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -735,45 +825,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -856,57 +907,6 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -925,41 +925,41 @@
   <autoFilter ref="A1:AN25" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}"/>
   <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{5E4BCC7B-BD3D-4850-9D02-5BDA26FED269}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{CA31088B-0A58-4A64-AE47-76C708B3947A}" name="NORTE" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{49129A23-8E4D-43BD-A688-921DB22B8F95}" name="RR" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{A165E71E-265F-4003-AA0E-8E9F26D12909}" name="RO" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{A386A7C6-C111-4CC7-8C16-FD58B8F0562F}" name="AC" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{9B733D29-A480-4FD0-A166-98AAD1AC2E74}" name="AM" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{F2B3378A-D467-452B-B894-8576A5D41BBE}" name="AP" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{2FE38FD4-49A7-402E-9249-2F1FE7E4E027}" name="PA" dataDxfId="98"/>
-    <tableColumn id="9" xr3:uid="{3F8DA4DF-43C6-4A2E-9793-6FB45F31D88A}" name="TO" dataDxfId="97"/>
-    <tableColumn id="10" xr3:uid="{08FE1121-488E-4A8A-A1D0-3D0D87153D95}" name="NORDESTE" dataDxfId="96"/>
-    <tableColumn id="11" xr3:uid="{DD9EA0BE-AEB8-4904-BE5A-81EC4F42E4C6}" name="MA" dataDxfId="95"/>
-    <tableColumn id="12" xr3:uid="{C65CE50B-DF9F-4EFE-AC1E-19A16468713A}" name="PI" dataDxfId="94"/>
-    <tableColumn id="13" xr3:uid="{5D05969A-E1C7-43A7-B71B-22268FB3E232}" name="CE" dataDxfId="93"/>
-    <tableColumn id="14" xr3:uid="{A97B6897-CFFE-4661-B611-B2D60CCF0ADC}" name="RN" dataDxfId="92"/>
-    <tableColumn id="15" xr3:uid="{BF86C9D2-5807-4F40-9051-7A67068281AA}" name="PB" dataDxfId="91"/>
-    <tableColumn id="16" xr3:uid="{E3A30C52-12FA-4308-ACA5-E511229E5D56}" name="PE" dataDxfId="90"/>
-    <tableColumn id="17" xr3:uid="{986578B0-2D30-422D-AE94-C704D371A9ED}" name="AL" dataDxfId="89"/>
-    <tableColumn id="18" xr3:uid="{61435B55-D3FE-4C3A-812E-CE5D0118E63E}" name="SE" dataDxfId="88"/>
-    <tableColumn id="19" xr3:uid="{534969DF-1823-4F20-A806-97162E402F0E}" name="BA" dataDxfId="87"/>
-    <tableColumn id="20" xr3:uid="{EDE8B247-4C19-4366-8800-9FEBEE13F9EA}" name="CENTRO-OESTE" dataDxfId="86"/>
-    <tableColumn id="21" xr3:uid="{A1667BB6-B217-492E-ACA4-B6E7FA0AF37B}" name="MT" dataDxfId="85"/>
-    <tableColumn id="22" xr3:uid="{54601504-468E-416E-8E4D-408050EFD8F1}" name="MS" dataDxfId="84"/>
-    <tableColumn id="23" xr3:uid="{1CA71861-8B72-40F9-8803-77B24A439D3B}" name="GO" dataDxfId="83"/>
-    <tableColumn id="24" xr3:uid="{D65A4ED9-4AA6-46B6-85F9-FF04865D9CD9}" name="DF" dataDxfId="82"/>
-    <tableColumn id="25" xr3:uid="{84502B60-EABA-40A0-98B8-19B8961F1D37}" name="SUDESTE" dataDxfId="81"/>
-    <tableColumn id="26" xr3:uid="{B60F76A8-80E5-4C5C-9541-1F844E7A3AE1}" name="MG" dataDxfId="80"/>
-    <tableColumn id="27" xr3:uid="{CC4AA6A5-83E1-4E87-A2CC-245EF4F57BFB}" name="ES" dataDxfId="79"/>
-    <tableColumn id="28" xr3:uid="{CA5AB65D-6CEA-4F12-93CA-75E3666C2354}" name="RJ" dataDxfId="78"/>
-    <tableColumn id="29" xr3:uid="{1E391A6D-FDCF-41F4-8790-26376C8AD795}" name="SP" dataDxfId="77"/>
-    <tableColumn id="30" xr3:uid="{04C869B7-96FC-43E9-9CE2-82769EFFDCA0}" name="SUL" dataDxfId="76"/>
-    <tableColumn id="31" xr3:uid="{9DCC0D0C-ACE3-4E6C-966D-A3E9ED01FBB5}" name="PR" dataDxfId="75"/>
-    <tableColumn id="32" xr3:uid="{C1056F8D-2C9F-4314-8424-F2B642B3F545}" name="SC" dataDxfId="74"/>
-    <tableColumn id="33" xr3:uid="{417BD3DD-D799-4503-A0AE-70D3CF2E75F7}" name="RS" dataDxfId="73"/>
-    <tableColumn id="34" xr3:uid="{E9B9638C-63FC-4E3C-9765-611D2BA02CEF}" name="NORTE-NORDESTE" dataDxfId="72"/>
-    <tableColumn id="35" xr3:uid="{BB0E374F-8FC9-4AE4-A4A2-6F762AEF1580}" name="CENTRO-SUL" dataDxfId="71"/>
-    <tableColumn id="36" xr3:uid="{8C7BDB00-4B75-4FF9-8F29-D37982132B90}" name="BRASIL" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{CA31088B-0A58-4A64-AE47-76C708B3947A}" name="NORTE" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{49129A23-8E4D-43BD-A688-921DB22B8F95}" name="RR" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{A165E71E-265F-4003-AA0E-8E9F26D12909}" name="RO" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{A386A7C6-C111-4CC7-8C16-FD58B8F0562F}" name="AC" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{9B733D29-A480-4FD0-A166-98AAD1AC2E74}" name="AM" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{F2B3378A-D467-452B-B894-8576A5D41BBE}" name="AP" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{2FE38FD4-49A7-402E-9249-2F1FE7E4E027}" name="PA" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{3F8DA4DF-43C6-4A2E-9793-6FB45F31D88A}" name="TO" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{08FE1121-488E-4A8A-A1D0-3D0D87153D95}" name="NORDESTE" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{DD9EA0BE-AEB8-4904-BE5A-81EC4F42E4C6}" name="MA" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{C65CE50B-DF9F-4EFE-AC1E-19A16468713A}" name="PI" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{5D05969A-E1C7-43A7-B71B-22268FB3E232}" name="CE" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{A97B6897-CFFE-4661-B611-B2D60CCF0ADC}" name="RN" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{BF86C9D2-5807-4F40-9051-7A67068281AA}" name="PB" dataDxfId="21"/>
+    <tableColumn id="16" xr3:uid="{E3A30C52-12FA-4308-ACA5-E511229E5D56}" name="PE" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{986578B0-2D30-422D-AE94-C704D371A9ED}" name="AL" dataDxfId="19"/>
+    <tableColumn id="18" xr3:uid="{61435B55-D3FE-4C3A-812E-CE5D0118E63E}" name="SE" dataDxfId="18"/>
+    <tableColumn id="19" xr3:uid="{534969DF-1823-4F20-A806-97162E402F0E}" name="BA" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{EDE8B247-4C19-4366-8800-9FEBEE13F9EA}" name="CENTRO-OESTE" dataDxfId="16"/>
+    <tableColumn id="21" xr3:uid="{A1667BB6-B217-492E-ACA4-B6E7FA0AF37B}" name="MT" dataDxfId="15"/>
+    <tableColumn id="22" xr3:uid="{54601504-468E-416E-8E4D-408050EFD8F1}" name="MS" dataDxfId="14"/>
+    <tableColumn id="23" xr3:uid="{1CA71861-8B72-40F9-8803-77B24A439D3B}" name="GO" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{D65A4ED9-4AA6-46B6-85F9-FF04865D9CD9}" name="DF" dataDxfId="12"/>
+    <tableColumn id="25" xr3:uid="{84502B60-EABA-40A0-98B8-19B8961F1D37}" name="SUDESTE" dataDxfId="11"/>
+    <tableColumn id="26" xr3:uid="{B60F76A8-80E5-4C5C-9541-1F844E7A3AE1}" name="MG" dataDxfId="10"/>
+    <tableColumn id="27" xr3:uid="{CC4AA6A5-83E1-4E87-A2CC-245EF4F57BFB}" name="ES" dataDxfId="9"/>
+    <tableColumn id="28" xr3:uid="{CA5AB65D-6CEA-4F12-93CA-75E3666C2354}" name="RJ" dataDxfId="8"/>
+    <tableColumn id="29" xr3:uid="{1E391A6D-FDCF-41F4-8790-26376C8AD795}" name="SP" dataDxfId="7"/>
+    <tableColumn id="30" xr3:uid="{04C869B7-96FC-43E9-9CE2-82769EFFDCA0}" name="SUL" dataDxfId="6"/>
+    <tableColumn id="31" xr3:uid="{9DCC0D0C-ACE3-4E6C-966D-A3E9ED01FBB5}" name="PR" dataDxfId="5"/>
+    <tableColumn id="32" xr3:uid="{C1056F8D-2C9F-4314-8424-F2B642B3F545}" name="SC" dataDxfId="4"/>
+    <tableColumn id="33" xr3:uid="{417BD3DD-D799-4503-A0AE-70D3CF2E75F7}" name="RS" dataDxfId="3"/>
+    <tableColumn id="34" xr3:uid="{E9B9638C-63FC-4E3C-9765-611D2BA02CEF}" name="NORTE-NORDESTE" dataDxfId="2"/>
+    <tableColumn id="35" xr3:uid="{BB0E374F-8FC9-4AE4-A4A2-6F762AEF1580}" name="CENTRO-SUL" dataDxfId="1"/>
+    <tableColumn id="36" xr3:uid="{8C7BDB00-4B75-4FF9-8F29-D37982132B90}" name="BRASIL" dataDxfId="0"/>
     <tableColumn id="37" xr3:uid="{0FF9F8EF-1643-4E16-A1B9-53905A2DD396}" name="ANO" dataDxfId="200"/>
     <tableColumn id="38" xr3:uid="{A4BC462C-3977-4A40-BE0D-1A25B4C47A2A}" name="MÊS" dataDxfId="199"/>
     <tableColumn id="39" xr3:uid="{8717C3B1-3F56-4A6D-8272-548CC6EE93AA}" name="SAFRA" dataDxfId="198"/>
@@ -974,45 +974,45 @@
   <autoFilter ref="A1:AN25" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}"/>
   <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{8CF1AF50-3446-4E75-8105-3A27A31DC53D}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{B84906ED-0B3E-4BAF-823C-613564EC7F44}" name="NORTE" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{84B9811A-583F-4CE3-B96E-FD8D3F9C0AF7}" name="RR" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{0AFF1D5D-3E87-4339-BBA1-770DC84997E0}" name="RO" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{8E7E000F-2618-4C1D-A0A3-786BAD1CCA1E}" name="AC" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{8FDC185D-309C-44F0-909D-47D36E4E88C7}" name="AM" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{FCFBA294-1B56-4D43-81BD-8397D063FB54}" name="AP" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{A4D89CF5-1E5F-4A95-9E6F-6AF87D6DC899}" name="PA" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{CBEB4E66-65D5-43C3-A560-E78883927AF4}" name="TO" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{E7D25C84-64C7-44D2-85A6-1289EF929C61}" name="NORDESTE" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{3A9FA498-3724-4EB1-92DC-966AAB9D214D}" name="MA" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{217BE2AA-49BC-4EFB-A2E9-A68DAFEE98F1}" name="PI" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{2A2F8CD6-E44E-48F7-95FF-898DA8413AFD}" name="CE" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{A6E9090C-1AB9-4D6E-9F99-ABDA730D9CA6}" name="RN" dataDxfId="57"/>
-    <tableColumn id="15" xr3:uid="{C74DAA05-C155-4F4D-B631-EB31FBB3665F}" name="PB" dataDxfId="56"/>
-    <tableColumn id="16" xr3:uid="{E5A10D15-FEE8-4661-ADBA-FB28CEA9267C}" name="PE" dataDxfId="55"/>
-    <tableColumn id="17" xr3:uid="{D1DA04F7-F9F0-4017-AE33-C5C1E7CE5AC0}" name="AL" dataDxfId="54"/>
-    <tableColumn id="18" xr3:uid="{DD2B9F5D-C570-466E-82CC-C54D2042ADFD}" name="SE" dataDxfId="53"/>
-    <tableColumn id="19" xr3:uid="{A2536CAA-3E99-4275-8AFB-0F230AD1FE08}" name="BA" dataDxfId="52"/>
-    <tableColumn id="20" xr3:uid="{C9DE622E-9653-49C4-97A9-6F44C0598F06}" name="CENTRO-OESTE" dataDxfId="51"/>
-    <tableColumn id="21" xr3:uid="{625EA772-B512-443B-A734-AF5CE77AB668}" name="MT" dataDxfId="50"/>
-    <tableColumn id="22" xr3:uid="{71A57575-7815-481F-AAAC-8C1EE9703912}" name="MS" dataDxfId="49"/>
-    <tableColumn id="23" xr3:uid="{F0365580-4820-46C6-A7D7-BD7C897237CB}" name="GO" dataDxfId="48"/>
-    <tableColumn id="24" xr3:uid="{A5D6C791-8D94-4B52-8C0C-39F7AD4AC4E1}" name="DF" dataDxfId="47"/>
-    <tableColumn id="25" xr3:uid="{3C464D88-F9B1-4C7A-8784-1840561093C3}" name="SUDESTE" dataDxfId="46"/>
-    <tableColumn id="26" xr3:uid="{1184085B-389F-4DFA-BAAA-79A73F5D58E9}" name="MG" dataDxfId="45"/>
-    <tableColumn id="27" xr3:uid="{1FD7AAC9-8B22-4599-8C41-97B306E682A8}" name="ES" dataDxfId="44"/>
-    <tableColumn id="28" xr3:uid="{3789E530-8644-46B9-A1D9-538F173953B6}" name="RJ" dataDxfId="43"/>
-    <tableColumn id="29" xr3:uid="{4B510379-3A08-42EB-8F76-653D7A9A0F0C}" name="SP" dataDxfId="42"/>
-    <tableColumn id="30" xr3:uid="{B7137113-AFD6-4F75-AE3E-0C0A27D770EB}" name="SUL" dataDxfId="41"/>
-    <tableColumn id="31" xr3:uid="{725B070C-B20E-4909-860C-25B32C284E06}" name="PR" dataDxfId="40"/>
-    <tableColumn id="32" xr3:uid="{4407D65F-AE79-48AC-9A84-33DCE4A2ADA4}" name="SC" dataDxfId="39"/>
-    <tableColumn id="33" xr3:uid="{88C455AC-C842-489F-84B2-E60D576F9F16}" name="RS" dataDxfId="38"/>
-    <tableColumn id="34" xr3:uid="{F04DD72A-4B16-4880-860B-5C4A2F256C93}" name="NORTE-NORDESTE" dataDxfId="37"/>
-    <tableColumn id="35" xr3:uid="{83D2B4A6-D70A-4652-89BB-1ED9B337F34A}" name="CENTRO-SUL" dataDxfId="36"/>
-    <tableColumn id="36" xr3:uid="{E90095A4-CB96-450E-A159-B808E8913751}" name="BRASIL" dataDxfId="35"/>
-    <tableColumn id="37" xr3:uid="{5796B11A-3AF2-4B43-92FF-178971C3DBD9}" name="ANO" dataDxfId="193"/>
-    <tableColumn id="38" xr3:uid="{5B4B4C2C-6AED-479F-B62E-92551DACC89D}" name="MÊS" dataDxfId="192"/>
-    <tableColumn id="39" xr3:uid="{453C9B87-B335-49FF-BF33-6444C74EE93B}" name="SAFRA" dataDxfId="191"/>
-    <tableColumn id="40" xr3:uid="{4C515472-E8FC-44F9-ACC7-A70C948FC297}" name="TIPO" dataDxfId="190"/>
+    <tableColumn id="2" xr3:uid="{B84906ED-0B3E-4BAF-823C-613564EC7F44}" name="NORTE" dataDxfId="196"/>
+    <tableColumn id="3" xr3:uid="{84B9811A-583F-4CE3-B96E-FD8D3F9C0AF7}" name="RR" dataDxfId="195"/>
+    <tableColumn id="4" xr3:uid="{0AFF1D5D-3E87-4339-BBA1-770DC84997E0}" name="RO" dataDxfId="194"/>
+    <tableColumn id="5" xr3:uid="{8E7E000F-2618-4C1D-A0A3-786BAD1CCA1E}" name="AC" dataDxfId="193"/>
+    <tableColumn id="6" xr3:uid="{8FDC185D-309C-44F0-909D-47D36E4E88C7}" name="AM" dataDxfId="192"/>
+    <tableColumn id="7" xr3:uid="{FCFBA294-1B56-4D43-81BD-8397D063FB54}" name="AP" dataDxfId="191"/>
+    <tableColumn id="8" xr3:uid="{A4D89CF5-1E5F-4A95-9E6F-6AF87D6DC899}" name="PA" dataDxfId="190"/>
+    <tableColumn id="9" xr3:uid="{CBEB4E66-65D5-43C3-A560-E78883927AF4}" name="TO" dataDxfId="189"/>
+    <tableColumn id="10" xr3:uid="{E7D25C84-64C7-44D2-85A6-1289EF929C61}" name="NORDESTE" dataDxfId="188"/>
+    <tableColumn id="11" xr3:uid="{3A9FA498-3724-4EB1-92DC-966AAB9D214D}" name="MA" dataDxfId="187"/>
+    <tableColumn id="12" xr3:uid="{217BE2AA-49BC-4EFB-A2E9-A68DAFEE98F1}" name="PI" dataDxfId="186"/>
+    <tableColumn id="13" xr3:uid="{2A2F8CD6-E44E-48F7-95FF-898DA8413AFD}" name="CE" dataDxfId="185"/>
+    <tableColumn id="14" xr3:uid="{A6E9090C-1AB9-4D6E-9F99-ABDA730D9CA6}" name="RN" dataDxfId="184"/>
+    <tableColumn id="15" xr3:uid="{C74DAA05-C155-4F4D-B631-EB31FBB3665F}" name="PB" dataDxfId="183"/>
+    <tableColumn id="16" xr3:uid="{E5A10D15-FEE8-4661-ADBA-FB28CEA9267C}" name="PE" dataDxfId="182"/>
+    <tableColumn id="17" xr3:uid="{D1DA04F7-F9F0-4017-AE33-C5C1E7CE5AC0}" name="AL" dataDxfId="181"/>
+    <tableColumn id="18" xr3:uid="{DD2B9F5D-C570-466E-82CC-C54D2042ADFD}" name="SE" dataDxfId="180"/>
+    <tableColumn id="19" xr3:uid="{A2536CAA-3E99-4275-8AFB-0F230AD1FE08}" name="BA" dataDxfId="179"/>
+    <tableColumn id="20" xr3:uid="{C9DE622E-9653-49C4-97A9-6F44C0598F06}" name="CENTRO-OESTE" dataDxfId="178"/>
+    <tableColumn id="21" xr3:uid="{625EA772-B512-443B-A734-AF5CE77AB668}" name="MT" dataDxfId="177"/>
+    <tableColumn id="22" xr3:uid="{71A57575-7815-481F-AAAC-8C1EE9703912}" name="MS" dataDxfId="176"/>
+    <tableColumn id="23" xr3:uid="{F0365580-4820-46C6-A7D7-BD7C897237CB}" name="GO" dataDxfId="175"/>
+    <tableColumn id="24" xr3:uid="{A5D6C791-8D94-4B52-8C0C-39F7AD4AC4E1}" name="DF" dataDxfId="174"/>
+    <tableColumn id="25" xr3:uid="{3C464D88-F9B1-4C7A-8784-1840561093C3}" name="SUDESTE" dataDxfId="173"/>
+    <tableColumn id="26" xr3:uid="{1184085B-389F-4DFA-BAAA-79A73F5D58E9}" name="MG" dataDxfId="172"/>
+    <tableColumn id="27" xr3:uid="{1FD7AAC9-8B22-4599-8C41-97B306E682A8}" name="ES" dataDxfId="171"/>
+    <tableColumn id="28" xr3:uid="{3789E530-8644-46B9-A1D9-538F173953B6}" name="RJ" dataDxfId="170"/>
+    <tableColumn id="29" xr3:uid="{4B510379-3A08-42EB-8F76-653D7A9A0F0C}" name="SP" dataDxfId="169"/>
+    <tableColumn id="30" xr3:uid="{B7137113-AFD6-4F75-AE3E-0C0A27D770EB}" name="SUL" dataDxfId="168"/>
+    <tableColumn id="31" xr3:uid="{725B070C-B20E-4909-860C-25B32C284E06}" name="PR" dataDxfId="167"/>
+    <tableColumn id="32" xr3:uid="{4407D65F-AE79-48AC-9A84-33DCE4A2ADA4}" name="SC" dataDxfId="166"/>
+    <tableColumn id="33" xr3:uid="{88C455AC-C842-489F-84B2-E60D576F9F16}" name="RS" dataDxfId="165"/>
+    <tableColumn id="34" xr3:uid="{F04DD72A-4B16-4880-860B-5C4A2F256C93}" name="NORTE-NORDESTE" dataDxfId="164"/>
+    <tableColumn id="35" xr3:uid="{83D2B4A6-D70A-4652-89BB-1ED9B337F34A}" name="CENTRO-SUL" dataDxfId="163"/>
+    <tableColumn id="36" xr3:uid="{E90095A4-CB96-450E-A159-B808E8913751}" name="BRASIL" dataDxfId="162"/>
+    <tableColumn id="37" xr3:uid="{5796B11A-3AF2-4B43-92FF-178971C3DBD9}" name="ANO" dataDxfId="161"/>
+    <tableColumn id="38" xr3:uid="{5B4B4C2C-6AED-479F-B62E-92551DACC89D}" name="MÊS" dataDxfId="160"/>
+    <tableColumn id="39" xr3:uid="{453C9B87-B335-49FF-BF33-6444C74EE93B}" name="SAFRA" dataDxfId="159"/>
+    <tableColumn id="40" xr3:uid="{4C515472-E8FC-44F9-ACC7-A70C948FC297}" name="TIPO" dataDxfId="158"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1023,45 +1023,45 @@
   <autoFilter ref="A1:AN25" xr:uid="{F205EC7A-49EF-4699-9240-6A619C4E0678}"/>
   <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{6051C5E2-E2B7-4BEB-BC76-2DCAA50A7C15}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{B8D0D550-3F4A-455D-B730-DC7BB52A9B2A}" name="NORTE" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{F0C3B647-0AA7-4BDE-9C13-1E481DDA789C}" name="RR" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{2118BB87-FCC8-403D-8FCA-D68B9ED42B8C}" name="RO" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{3CA4EDC5-768A-430C-8DF0-0D22D3452853}" name="AC" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{7362E812-6294-4692-A499-A02354A455C2}" name="AM" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{482DE189-3576-4B8E-BF1A-9C58B5F5C6ED}" name="AP" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{0E0FA7BD-E6EA-426B-B8B1-9665A67EE819}" name="PA" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{9ABF8262-0C59-4BAA-8D66-6D70743CECED}" name="TO" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{96D8ACAF-FFFE-4005-ADC1-94AA97CD6038}" name="NORDESTE" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{1FABF4C2-AC99-4575-B4A2-682FB02C27AB}" name="MA" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{6E7000A1-CF81-4A5C-AF79-B5A606493E58}" name="PI" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{5804C6F2-0132-4A60-8701-6454E76B39E1}" name="CE" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{FAC246D4-9925-4737-BA6E-C12890CC3492}" name="RN" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{70365A79-11D8-4822-868C-B390282D31AA}" name="PB" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{C5EA46D4-2A74-4A1B-8628-EDE27732EBC1}" name="PE" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{3AB16384-A9C1-4EAE-B1D3-B6980668DDFB}" name="AL" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{5550B480-640D-47F3-98E2-47360C39B350}" name="SE" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{AC7410A2-BEC3-4F36-9DE3-007ABEDAFE77}" name="BA" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{EF9CC834-4DE2-4F12-A01F-E188C35BB745}" name="CENTRO-OESTE" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{43361983-B660-4F10-8172-158B7FE088A3}" name="MT" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{1D87111A-4709-4B48-BC75-F06DA78D87CB}" name="MS" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{8C8B08DD-2483-4E25-AB6C-69DC01B3EB3D}" name="GO" dataDxfId="13"/>
-    <tableColumn id="24" xr3:uid="{9D3A4E55-E1CC-4509-9BBA-1BA1B5720931}" name="DF" dataDxfId="12"/>
-    <tableColumn id="25" xr3:uid="{64CEA2A0-9627-43CF-9192-24F44872CC96}" name="SUDESTE" dataDxfId="11"/>
-    <tableColumn id="26" xr3:uid="{4FBE3EC3-154E-4DF3-ABB6-B6DEFFC26271}" name="MG" dataDxfId="10"/>
-    <tableColumn id="27" xr3:uid="{B6B47D99-4133-4D01-BF64-2BBBE6D3BE49}" name="ES" dataDxfId="9"/>
-    <tableColumn id="28" xr3:uid="{7CC112A7-D0E8-4317-B401-EC4CD011155C}" name="RJ" dataDxfId="8"/>
-    <tableColumn id="29" xr3:uid="{14E6FF96-46F0-467D-A5A3-F1C831072AA9}" name="SP" dataDxfId="7"/>
-    <tableColumn id="30" xr3:uid="{932BDB91-3454-40CD-B097-52A8AA0A2F81}" name="SUL" dataDxfId="6"/>
-    <tableColumn id="31" xr3:uid="{AA858ED8-15B1-4985-9F57-E0EE2783C677}" name="PR" dataDxfId="5"/>
-    <tableColumn id="32" xr3:uid="{D302D227-008B-444D-87CF-C19499331330}" name="SC" dataDxfId="4"/>
-    <tableColumn id="33" xr3:uid="{65AB5642-25AB-4920-8029-D56BC42AB123}" name="RS" dataDxfId="3"/>
-    <tableColumn id="34" xr3:uid="{7666B84C-5946-494A-83CA-2B24D2CF0DC8}" name="NORTE-NORDESTE" dataDxfId="2"/>
-    <tableColumn id="35" xr3:uid="{633B8894-AE4A-45AC-B1C9-B4EAA702D9F9}" name="CENTRO-SUL" dataDxfId="1"/>
-    <tableColumn id="36" xr3:uid="{6BB08E62-BEF0-4192-83F6-2E12E9E586B8}" name="BRASIL" dataDxfId="0"/>
-    <tableColumn id="37" xr3:uid="{ECC44396-0C86-4DF0-B859-53097AD13988}" name="ANO" dataDxfId="186"/>
-    <tableColumn id="38" xr3:uid="{57AEF2DA-BFBE-4B5B-ABC0-477C4D3CA382}" name="MÊS" dataDxfId="185"/>
-    <tableColumn id="39" xr3:uid="{4AF1745A-E1C0-4A75-AFC1-E75F141DCCAA}" name="SAFRA" dataDxfId="184"/>
-    <tableColumn id="40" xr3:uid="{3CA074B3-E5CB-4769-955F-7E055E4BC613}" name="TIPO" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{B8D0D550-3F4A-455D-B730-DC7BB52A9B2A}" name="NORTE" dataDxfId="157"/>
+    <tableColumn id="3" xr3:uid="{F0C3B647-0AA7-4BDE-9C13-1E481DDA789C}" name="RR" dataDxfId="156"/>
+    <tableColumn id="4" xr3:uid="{2118BB87-FCC8-403D-8FCA-D68B9ED42B8C}" name="RO" dataDxfId="155"/>
+    <tableColumn id="5" xr3:uid="{3CA4EDC5-768A-430C-8DF0-0D22D3452853}" name="AC" dataDxfId="154"/>
+    <tableColumn id="6" xr3:uid="{7362E812-6294-4692-A499-A02354A455C2}" name="AM" dataDxfId="153"/>
+    <tableColumn id="7" xr3:uid="{482DE189-3576-4B8E-BF1A-9C58B5F5C6ED}" name="AP" dataDxfId="152"/>
+    <tableColumn id="8" xr3:uid="{0E0FA7BD-E6EA-426B-B8B1-9665A67EE819}" name="PA" dataDxfId="151"/>
+    <tableColumn id="9" xr3:uid="{9ABF8262-0C59-4BAA-8D66-6D70743CECED}" name="TO" dataDxfId="150"/>
+    <tableColumn id="10" xr3:uid="{96D8ACAF-FFFE-4005-ADC1-94AA97CD6038}" name="NORDESTE" dataDxfId="149"/>
+    <tableColumn id="11" xr3:uid="{1FABF4C2-AC99-4575-B4A2-682FB02C27AB}" name="MA" dataDxfId="148"/>
+    <tableColumn id="12" xr3:uid="{6E7000A1-CF81-4A5C-AF79-B5A606493E58}" name="PI" dataDxfId="147"/>
+    <tableColumn id="13" xr3:uid="{5804C6F2-0132-4A60-8701-6454E76B39E1}" name="CE" dataDxfId="146"/>
+    <tableColumn id="14" xr3:uid="{FAC246D4-9925-4737-BA6E-C12890CC3492}" name="RN" dataDxfId="145"/>
+    <tableColumn id="15" xr3:uid="{70365A79-11D8-4822-868C-B390282D31AA}" name="PB" dataDxfId="144"/>
+    <tableColumn id="16" xr3:uid="{C5EA46D4-2A74-4A1B-8628-EDE27732EBC1}" name="PE" dataDxfId="143"/>
+    <tableColumn id="17" xr3:uid="{3AB16384-A9C1-4EAE-B1D3-B6980668DDFB}" name="AL" dataDxfId="142"/>
+    <tableColumn id="18" xr3:uid="{5550B480-640D-47F3-98E2-47360C39B350}" name="SE" dataDxfId="141"/>
+    <tableColumn id="19" xr3:uid="{AC7410A2-BEC3-4F36-9DE3-007ABEDAFE77}" name="BA" dataDxfId="140"/>
+    <tableColumn id="20" xr3:uid="{EF9CC834-4DE2-4F12-A01F-E188C35BB745}" name="CENTRO-OESTE" dataDxfId="139"/>
+    <tableColumn id="21" xr3:uid="{43361983-B660-4F10-8172-158B7FE088A3}" name="MT" dataDxfId="138"/>
+    <tableColumn id="22" xr3:uid="{1D87111A-4709-4B48-BC75-F06DA78D87CB}" name="MS" dataDxfId="137"/>
+    <tableColumn id="23" xr3:uid="{8C8B08DD-2483-4E25-AB6C-69DC01B3EB3D}" name="GO" dataDxfId="136"/>
+    <tableColumn id="24" xr3:uid="{9D3A4E55-E1CC-4509-9BBA-1BA1B5720931}" name="DF" dataDxfId="135"/>
+    <tableColumn id="25" xr3:uid="{64CEA2A0-9627-43CF-9192-24F44872CC96}" name="SUDESTE" dataDxfId="134"/>
+    <tableColumn id="26" xr3:uid="{4FBE3EC3-154E-4DF3-ABB6-B6DEFFC26271}" name="MG" dataDxfId="133"/>
+    <tableColumn id="27" xr3:uid="{B6B47D99-4133-4D01-BF64-2BBBE6D3BE49}" name="ES" dataDxfId="132"/>
+    <tableColumn id="28" xr3:uid="{7CC112A7-D0E8-4317-B401-EC4CD011155C}" name="RJ" dataDxfId="131"/>
+    <tableColumn id="29" xr3:uid="{14E6FF96-46F0-467D-A5A3-F1C831072AA9}" name="SP" dataDxfId="130"/>
+    <tableColumn id="30" xr3:uid="{932BDB91-3454-40CD-B097-52A8AA0A2F81}" name="SUL" dataDxfId="129"/>
+    <tableColumn id="31" xr3:uid="{AA858ED8-15B1-4985-9F57-E0EE2783C677}" name="PR" dataDxfId="128"/>
+    <tableColumn id="32" xr3:uid="{D302D227-008B-444D-87CF-C19499331330}" name="SC" dataDxfId="127"/>
+    <tableColumn id="33" xr3:uid="{65AB5642-25AB-4920-8029-D56BC42AB123}" name="RS" dataDxfId="126"/>
+    <tableColumn id="34" xr3:uid="{7666B84C-5946-494A-83CA-2B24D2CF0DC8}" name="NORTE-NORDESTE" dataDxfId="125"/>
+    <tableColumn id="35" xr3:uid="{633B8894-AE4A-45AC-B1C9-B4EAA702D9F9}" name="CENTRO-SUL" dataDxfId="124"/>
+    <tableColumn id="36" xr3:uid="{6BB08E62-BEF0-4192-83F6-2E12E9E586B8}" name="BRASIL" dataDxfId="123"/>
+    <tableColumn id="37" xr3:uid="{ECC44396-0C86-4DF0-B859-53097AD13988}" name="ANO" dataDxfId="122"/>
+    <tableColumn id="38" xr3:uid="{57AEF2DA-BFBE-4B5B-ABC0-477C4D3CA382}" name="MÊS" dataDxfId="121"/>
+    <tableColumn id="39" xr3:uid="{4AF1745A-E1C0-4A75-AFC1-E75F141DCCAA}" name="SAFRA" dataDxfId="120"/>
+    <tableColumn id="40" xr3:uid="{3CA074B3-E5CB-4769-955F-7E055E4BC613}" name="TIPO" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1072,34 +1072,34 @@
   <autoFilter ref="A1:AC36" xr:uid="{6AAA68D2-2837-4E56-9205-588FBC25E607}"/>
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{9D8E11EB-62E4-4646-82D1-16F281AB841F}" name="REGIÃO"/>
-    <tableColumn id="2" xr3:uid="{400D5D9F-14BE-449D-A25E-F770F1684551}" name="ALGODÃO TOTAL" dataDxfId="179"/>
-    <tableColumn id="3" xr3:uid="{1A597964-8010-4331-ABEA-1AEA845AB5F5}" name="ALGODÃO PLUMA" dataDxfId="178"/>
-    <tableColumn id="4" xr3:uid="{B2BFD712-F833-47B4-830F-961CC061703C}" name="ALGODÃO CAROÇO" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{F4D73FDB-EAAE-4D0E-8E22-29A41F3B9E20}" name="AMENDOIM" dataDxfId="176"/>
-    <tableColumn id="6" xr3:uid="{5B9AB598-74CF-401E-9133-20988114821A}" name="ARROZ TOTAL" dataDxfId="175"/>
-    <tableColumn id="7" xr3:uid="{9F25F6FD-273B-47C9-A893-C8D4CAFE7AB6}" name="ARROZ SEQUEIRO" dataDxfId="174"/>
-    <tableColumn id="8" xr3:uid="{C5FEDFF2-6DFD-4C53-869F-F28A5C23DF3B}" name="ARROZ IRRIGADO" dataDxfId="173"/>
-    <tableColumn id="9" xr3:uid="{211D5550-928C-4A68-8D86-E36DF84B0861}" name="FEIJÃO TOTAL" dataDxfId="172"/>
-    <tableColumn id="10" xr3:uid="{9C00CC61-0B0F-43D5-A684-AE913448FB8D}" name="FEIJÃO CORES" dataDxfId="171"/>
-    <tableColumn id="11" xr3:uid="{F00934D7-9B86-45AA-8159-2128826AE03E}" name="FEIJÃO PRETO" dataDxfId="170"/>
-    <tableColumn id="12" xr3:uid="{1CBBEDAF-020E-4EFE-907A-27557665AA02}" name="FEIJÃO CAUPI" dataDxfId="169"/>
-    <tableColumn id="13" xr3:uid="{A8B4A0BB-9E8E-4F8C-9B7B-89F6D688EC32}" name="GERGELIM" dataDxfId="168"/>
-    <tableColumn id="14" xr3:uid="{BD44DF76-DF43-47F8-8A9E-050E54211B27}" name="GIRASSOL" dataDxfId="167"/>
-    <tableColumn id="15" xr3:uid="{E3E75921-B2B5-4327-9628-9461D4B2C97A}" name="MAMONA" dataDxfId="166"/>
-    <tableColumn id="16" xr3:uid="{779BE33D-35AA-4039-A599-BA68B482A978}" name="MILHO" dataDxfId="165"/>
-    <tableColumn id="17" xr3:uid="{AC0C1990-76E8-414D-951C-E60C4646E855}" name="SOJA" dataDxfId="164"/>
-    <tableColumn id="18" xr3:uid="{CC2AD535-2144-4A37-B30C-44803E8E0DC2}" name="SORGO" dataDxfId="163"/>
-    <tableColumn id="19" xr3:uid="{DB09C5E0-C39A-4FE3-A0C4-5F83F16E55BE}" name="AVEIA" dataDxfId="162"/>
-    <tableColumn id="20" xr3:uid="{A5A1A29D-945B-43C5-872F-5D7E2D8C0F4F}" name="CANOLA" dataDxfId="161"/>
-    <tableColumn id="21" xr3:uid="{07F643AF-5A03-40BB-B5E8-C02BD7E21808}" name="CENTEIO" dataDxfId="160"/>
-    <tableColumn id="22" xr3:uid="{6A47C86C-50FC-4E1C-8369-917038B220D3}" name="CEVADA" dataDxfId="159"/>
-    <tableColumn id="23" xr3:uid="{2D22156A-463D-4284-9CD8-69F0E87747E7}" name="TRIGO" dataDxfId="158"/>
-    <tableColumn id="24" xr3:uid="{5ACD3FF0-294A-44A8-8DF0-F447B6863725}" name="TRITICALE" dataDxfId="157"/>
-    <tableColumn id="25" xr3:uid="{E71C1FB1-73E6-456B-8624-C3377581DF94}" name="GERAL" dataDxfId="155"/>
-    <tableColumn id="26" xr3:uid="{8186BB93-C0FE-4341-A195-EA43AAD936F3}" name="ANO" dataDxfId="156"/>
-    <tableColumn id="27" xr3:uid="{87DB167D-5607-4997-951C-88947D3A6327}" name="MÊS" dataDxfId="196"/>
-    <tableColumn id="28" xr3:uid="{C07FA4E5-704A-4BBC-9B48-E235E6FEA795}" name="SAFRA" dataDxfId="195"/>
-    <tableColumn id="29" xr3:uid="{80D56BA8-F184-4BB6-A104-136DE9A59792}" name="TIPO" dataDxfId="194"/>
+    <tableColumn id="2" xr3:uid="{400D5D9F-14BE-449D-A25E-F770F1684551}" name="ALGODÃO TOTAL" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{1A597964-8010-4331-ABEA-1AEA845AB5F5}" name="ALGODÃO PLUMA" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{B2BFD712-F833-47B4-830F-961CC061703C}" name="ALGODÃO CAROÇO" dataDxfId="116"/>
+    <tableColumn id="5" xr3:uid="{F4D73FDB-EAAE-4D0E-8E22-29A41F3B9E20}" name="AMENDOIM" dataDxfId="115"/>
+    <tableColumn id="6" xr3:uid="{5B9AB598-74CF-401E-9133-20988114821A}" name="ARROZ TOTAL" dataDxfId="114"/>
+    <tableColumn id="7" xr3:uid="{9F25F6FD-273B-47C9-A893-C8D4CAFE7AB6}" name="ARROZ SEQUEIRO" dataDxfId="113"/>
+    <tableColumn id="8" xr3:uid="{C5FEDFF2-6DFD-4C53-869F-F28A5C23DF3B}" name="ARROZ IRRIGADO" dataDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{211D5550-928C-4A68-8D86-E36DF84B0861}" name="FEIJÃO TOTAL" dataDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{9C00CC61-0B0F-43D5-A684-AE913448FB8D}" name="FEIJÃO CORES" dataDxfId="110"/>
+    <tableColumn id="11" xr3:uid="{F00934D7-9B86-45AA-8159-2128826AE03E}" name="FEIJÃO PRETO" dataDxfId="109"/>
+    <tableColumn id="12" xr3:uid="{1CBBEDAF-020E-4EFE-907A-27557665AA02}" name="FEIJÃO CAUPI" dataDxfId="108"/>
+    <tableColumn id="13" xr3:uid="{A8B4A0BB-9E8E-4F8C-9B7B-89F6D688EC32}" name="GERGELIM" dataDxfId="107"/>
+    <tableColumn id="14" xr3:uid="{BD44DF76-DF43-47F8-8A9E-050E54211B27}" name="GIRASSOL" dataDxfId="106"/>
+    <tableColumn id="15" xr3:uid="{E3E75921-B2B5-4327-9628-9461D4B2C97A}" name="MAMONA" dataDxfId="105"/>
+    <tableColumn id="16" xr3:uid="{779BE33D-35AA-4039-A599-BA68B482A978}" name="MILHO" dataDxfId="104"/>
+    <tableColumn id="17" xr3:uid="{AC0C1990-76E8-414D-951C-E60C4646E855}" name="SOJA" dataDxfId="103"/>
+    <tableColumn id="18" xr3:uid="{CC2AD535-2144-4A37-B30C-44803E8E0DC2}" name="SORGO" dataDxfId="102"/>
+    <tableColumn id="19" xr3:uid="{DB09C5E0-C39A-4FE3-A0C4-5F83F16E55BE}" name="AVEIA" dataDxfId="101"/>
+    <tableColumn id="20" xr3:uid="{A5A1A29D-945B-43C5-872F-5D7E2D8C0F4F}" name="CANOLA" dataDxfId="100"/>
+    <tableColumn id="21" xr3:uid="{07F643AF-5A03-40BB-B5E8-C02BD7E21808}" name="CENTEIO" dataDxfId="99"/>
+    <tableColumn id="22" xr3:uid="{6A47C86C-50FC-4E1C-8369-917038B220D3}" name="CEVADA" dataDxfId="98"/>
+    <tableColumn id="23" xr3:uid="{2D22156A-463D-4284-9CD8-69F0E87747E7}" name="TRIGO" dataDxfId="97"/>
+    <tableColumn id="24" xr3:uid="{5ACD3FF0-294A-44A8-8DF0-F447B6863725}" name="TRITICALE" dataDxfId="96"/>
+    <tableColumn id="25" xr3:uid="{E71C1FB1-73E6-456B-8624-C3377581DF94}" name="GERAL" dataDxfId="95"/>
+    <tableColumn id="26" xr3:uid="{8186BB93-C0FE-4341-A195-EA43AAD936F3}" name="ANO" dataDxfId="94"/>
+    <tableColumn id="27" xr3:uid="{87DB167D-5607-4997-951C-88947D3A6327}" name="MÊS" dataDxfId="93"/>
+    <tableColumn id="28" xr3:uid="{C07FA4E5-704A-4BBC-9B48-E235E6FEA795}" name="SAFRA" dataDxfId="92"/>
+    <tableColumn id="29" xr3:uid="{80D56BA8-F184-4BB6-A104-136DE9A59792}" name="TIPO" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1110,34 +1110,34 @@
   <autoFilter ref="A1:AC36" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}"/>
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{DAF3B878-FB08-46CD-ACA1-18181EFBFBAD}" name="REGIÃO"/>
-    <tableColumn id="2" xr3:uid="{696769AD-331A-446B-8AC3-B7C2D6DFB4E8}" name="ALGODÃO TOTAL" dataDxfId="154"/>
-    <tableColumn id="3" xr3:uid="{5E665A64-E5CA-4198-9ED1-223E0FFF8B1A}" name="ALGODÃO PLUMA" dataDxfId="153"/>
-    <tableColumn id="4" xr3:uid="{57ADDDDD-9A37-44E9-983C-5B9F0D61AF11}" name="ALGODÃO CAROÇO" dataDxfId="152"/>
-    <tableColumn id="5" xr3:uid="{BD6D0D9E-BA32-4F0C-BAA5-432806AD0AA9}" name="AMENDOIM" dataDxfId="151"/>
-    <tableColumn id="6" xr3:uid="{C681D5C9-AA19-42EE-BA4D-84A974B167AB}" name="ARROZ TOTAL" dataDxfId="150"/>
-    <tableColumn id="7" xr3:uid="{21C89C02-6582-4EA1-885A-BE6F358EFB65}" name="ARROZ SEQUEIRO" dataDxfId="149"/>
-    <tableColumn id="8" xr3:uid="{501ED1B5-AC3F-4814-A140-66E033D4A6D8}" name="ARROZ IRRIGADO" dataDxfId="148"/>
-    <tableColumn id="9" xr3:uid="{04AD2B17-EAE9-468E-9CE2-F9622EDD8FAB}" name="FEIJÃO TOTAL" dataDxfId="147"/>
-    <tableColumn id="10" xr3:uid="{42CBB38A-7B8E-4D57-921D-C225BD11BA37}" name="FEIJÃO CORES" dataDxfId="146"/>
-    <tableColumn id="11" xr3:uid="{2D91C5A5-E4B0-489B-803D-F2729F4C4F74}" name="FEIJÃO PRETO" dataDxfId="145"/>
-    <tableColumn id="12" xr3:uid="{99C1F29D-95F7-4EEA-8358-7E1C3C68D9BD}" name="FEIJÃO CAUPI" dataDxfId="144"/>
-    <tableColumn id="13" xr3:uid="{B56D35BC-0CE8-4B2C-AA42-0F259574BA42}" name="GERGELIM" dataDxfId="143"/>
-    <tableColumn id="14" xr3:uid="{DCA5F91F-E4C7-409B-8D7D-D7CB01BD5BD4}" name="GIRASSOL" dataDxfId="142"/>
-    <tableColumn id="15" xr3:uid="{C4FEE6B7-7EF6-456E-B8DE-D28E6D59FC75}" name="MAMONA" dataDxfId="141"/>
-    <tableColumn id="16" xr3:uid="{1355C0D1-26AC-4CDD-97CF-BBF69AC27943}" name="MILHO" dataDxfId="140"/>
-    <tableColumn id="17" xr3:uid="{F87E309F-FB19-4F9B-AF8A-791408964512}" name="SOJA" dataDxfId="139"/>
-    <tableColumn id="18" xr3:uid="{C3B3364B-EC9C-4949-8747-10B77423825C}" name="SORGO" dataDxfId="138"/>
-    <tableColumn id="19" xr3:uid="{24AFF494-F277-42E7-BB5C-7D4DD4610D0A}" name="AVEIA" dataDxfId="137"/>
-    <tableColumn id="20" xr3:uid="{AA50ABAF-470B-4E78-B762-C184C2002B38}" name="CANOLA" dataDxfId="136"/>
-    <tableColumn id="21" xr3:uid="{E41B718D-8512-4FBA-94E7-68D66488A5A3}" name="CENTEIO" dataDxfId="135"/>
-    <tableColumn id="22" xr3:uid="{5FD3C437-7E82-475D-BB2A-21A8CCFB39A8}" name="CEVADA" dataDxfId="134"/>
-    <tableColumn id="23" xr3:uid="{521DED51-CA6F-48F2-89ED-A38C0B449C5F}" name="TRIGO" dataDxfId="133"/>
-    <tableColumn id="24" xr3:uid="{C71EED0F-A05C-4902-876D-30647F78380D}" name="TRITICALE" dataDxfId="132"/>
-    <tableColumn id="25" xr3:uid="{43F11742-31FE-47CA-9206-DE9A85BDFA19}" name="GERAL" dataDxfId="130"/>
-    <tableColumn id="26" xr3:uid="{C21B5348-2002-46F8-AF76-43C13BCC151D}" name="ANO" dataDxfId="131"/>
-    <tableColumn id="27" xr3:uid="{D891F035-96D6-480F-919B-B57924EE851E}" name="MÊS" dataDxfId="189"/>
-    <tableColumn id="28" xr3:uid="{0232FBA8-C0E4-432C-A673-68FECC15080F}" name="SAFRA" dataDxfId="188"/>
-    <tableColumn id="29" xr3:uid="{34339AE0-605D-4295-9A38-48ED61D0BFC6}" name="TIPO" dataDxfId="187"/>
+    <tableColumn id="2" xr3:uid="{696769AD-331A-446B-8AC3-B7C2D6DFB4E8}" name="ALGODÃO TOTAL" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{5E665A64-E5CA-4198-9ED1-223E0FFF8B1A}" name="ALGODÃO PLUMA" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{57ADDDDD-9A37-44E9-983C-5B9F0D61AF11}" name="ALGODÃO CAROÇO" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{BD6D0D9E-BA32-4F0C-BAA5-432806AD0AA9}" name="AMENDOIM" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{C681D5C9-AA19-42EE-BA4D-84A974B167AB}" name="ARROZ TOTAL" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{21C89C02-6582-4EA1-885A-BE6F358EFB65}" name="ARROZ SEQUEIRO" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{501ED1B5-AC3F-4814-A140-66E033D4A6D8}" name="ARROZ IRRIGADO" dataDxfId="84"/>
+    <tableColumn id="9" xr3:uid="{04AD2B17-EAE9-468E-9CE2-F9622EDD8FAB}" name="FEIJÃO TOTAL" dataDxfId="83"/>
+    <tableColumn id="10" xr3:uid="{42CBB38A-7B8E-4D57-921D-C225BD11BA37}" name="FEIJÃO CORES" dataDxfId="82"/>
+    <tableColumn id="11" xr3:uid="{2D91C5A5-E4B0-489B-803D-F2729F4C4F74}" name="FEIJÃO PRETO" dataDxfId="81"/>
+    <tableColumn id="12" xr3:uid="{99C1F29D-95F7-4EEA-8358-7E1C3C68D9BD}" name="FEIJÃO CAUPI" dataDxfId="80"/>
+    <tableColumn id="13" xr3:uid="{B56D35BC-0CE8-4B2C-AA42-0F259574BA42}" name="GERGELIM" dataDxfId="79"/>
+    <tableColumn id="14" xr3:uid="{DCA5F91F-E4C7-409B-8D7D-D7CB01BD5BD4}" name="GIRASSOL" dataDxfId="78"/>
+    <tableColumn id="15" xr3:uid="{C4FEE6B7-7EF6-456E-B8DE-D28E6D59FC75}" name="MAMONA" dataDxfId="77"/>
+    <tableColumn id="16" xr3:uid="{1355C0D1-26AC-4CDD-97CF-BBF69AC27943}" name="MILHO" dataDxfId="76"/>
+    <tableColumn id="17" xr3:uid="{F87E309F-FB19-4F9B-AF8A-791408964512}" name="SOJA" dataDxfId="75"/>
+    <tableColumn id="18" xr3:uid="{C3B3364B-EC9C-4949-8747-10B77423825C}" name="SORGO" dataDxfId="74"/>
+    <tableColumn id="19" xr3:uid="{24AFF494-F277-42E7-BB5C-7D4DD4610D0A}" name="AVEIA" dataDxfId="73"/>
+    <tableColumn id="20" xr3:uid="{AA50ABAF-470B-4E78-B762-C184C2002B38}" name="CANOLA" dataDxfId="72"/>
+    <tableColumn id="21" xr3:uid="{E41B718D-8512-4FBA-94E7-68D66488A5A3}" name="CENTEIO" dataDxfId="71"/>
+    <tableColumn id="22" xr3:uid="{5FD3C437-7E82-475D-BB2A-21A8CCFB39A8}" name="CEVADA" dataDxfId="70"/>
+    <tableColumn id="23" xr3:uid="{521DED51-CA6F-48F2-89ED-A38C0B449C5F}" name="TRIGO" dataDxfId="69"/>
+    <tableColumn id="24" xr3:uid="{C71EED0F-A05C-4902-876D-30647F78380D}" name="TRITICALE" dataDxfId="68"/>
+    <tableColumn id="25" xr3:uid="{43F11742-31FE-47CA-9206-DE9A85BDFA19}" name="GERAL" dataDxfId="67"/>
+    <tableColumn id="26" xr3:uid="{C21B5348-2002-46F8-AF76-43C13BCC151D}" name="ANO" dataDxfId="66"/>
+    <tableColumn id="27" xr3:uid="{D891F035-96D6-480F-919B-B57924EE851E}" name="MÊS" dataDxfId="65"/>
+    <tableColumn id="28" xr3:uid="{0232FBA8-C0E4-432C-A673-68FECC15080F}" name="SAFRA" dataDxfId="64"/>
+    <tableColumn id="29" xr3:uid="{34339AE0-605D-4295-9A38-48ED61D0BFC6}" name="TIPO" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1148,34 +1148,34 @@
   <autoFilter ref="A1:AC36" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}"/>
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{97EFA303-A9FC-46C0-A365-D8BFD6B07F4E}" name="REGIÃO"/>
-    <tableColumn id="2" xr3:uid="{CD1BE27C-2122-4E57-BF75-B4E0FA407680}" name="ALGODÃO TOTAL" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{6AAC4787-45BB-49C3-925E-EB86773D0EE3}" name="ALGODÃO PLUMA" dataDxfId="128"/>
-    <tableColumn id="4" xr3:uid="{A709C33E-0EFD-439D-AFA6-DCBE5DFECC09}" name="ALGODÃO CAROÇO" dataDxfId="127"/>
-    <tableColumn id="5" xr3:uid="{36919ACC-6DBD-4BA6-B171-C06771CAA181}" name="AMENDOIM" dataDxfId="126"/>
-    <tableColumn id="6" xr3:uid="{A9E1ECF8-9280-4528-BB2D-F3444CC4E573}" name="ARROZ TOTAL" dataDxfId="125"/>
-    <tableColumn id="7" xr3:uid="{E24CCEF1-19C6-4E7E-8519-F2CBD6FFBD2C}" name="ARROZ SEQUEIRO" dataDxfId="124"/>
-    <tableColumn id="8" xr3:uid="{27262FD4-F510-4739-AE4D-503E89394540}" name="ARROZ IRRIGADO" dataDxfId="123"/>
-    <tableColumn id="9" xr3:uid="{07A828EE-65C2-453C-98A5-132A6F8EEB49}" name="FEIJÃO TOTAL" dataDxfId="122"/>
-    <tableColumn id="10" xr3:uid="{77436711-59D7-4D39-A13D-93314192FF57}" name="FEIJÃO CORES" dataDxfId="121"/>
-    <tableColumn id="11" xr3:uid="{C39CBBE1-C887-4FAA-B20D-BEF14F189268}" name="FEIJÃO PRETO" dataDxfId="120"/>
-    <tableColumn id="12" xr3:uid="{793D8F4C-ED63-45E7-81EC-8827A45470EF}" name="FEIJÃO CAUPI" dataDxfId="119"/>
-    <tableColumn id="13" xr3:uid="{59CC00D7-C96D-4832-9F17-68AA9395C332}" name="GERGELIM" dataDxfId="118"/>
-    <tableColumn id="14" xr3:uid="{6F397307-9E9A-4B49-89A4-0D105DC65A10}" name="GIRASSOL" dataDxfId="117"/>
-    <tableColumn id="15" xr3:uid="{76D545D2-CB23-48DD-AB8A-DAF6093C755D}" name="MAMONA" dataDxfId="116"/>
-    <tableColumn id="16" xr3:uid="{72E88D52-C6D2-4CF2-8498-8A5F1E83E6C7}" name="MILHO" dataDxfId="115"/>
-    <tableColumn id="17" xr3:uid="{4972AB7E-DAFC-42EA-8460-6CE3DFB48C04}" name="SOJA" dataDxfId="114"/>
-    <tableColumn id="18" xr3:uid="{C27C81AD-E84C-4DB4-9290-8E1075D91C93}" name="SORGO" dataDxfId="113"/>
-    <tableColumn id="19" xr3:uid="{0A447A82-E343-410A-8854-08B23C052F47}" name="AVEIA" dataDxfId="112"/>
-    <tableColumn id="20" xr3:uid="{F5ED3C8B-B7CB-452E-96A2-FCCEB899C54E}" name="CANOLA" dataDxfId="111"/>
-    <tableColumn id="21" xr3:uid="{17829594-1EEC-4783-9488-1309944A44E5}" name="CENTEIO" dataDxfId="110"/>
-    <tableColumn id="22" xr3:uid="{49B2C1E3-0396-4037-BB4B-32C18FDB6CC7}" name="CEVADA" dataDxfId="109"/>
-    <tableColumn id="23" xr3:uid="{C10C34AB-D106-4FB2-B097-C90EF653E9E5}" name="TRIGO" dataDxfId="108"/>
-    <tableColumn id="24" xr3:uid="{80045204-E6E2-42D6-9449-CCD3B9641988}" name="TRITICALE" dataDxfId="107"/>
-    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="105"/>
-    <tableColumn id="26" xr3:uid="{FA0650E0-02EE-433A-927B-8DCFAD627C43}" name="ANO" dataDxfId="106"/>
-    <tableColumn id="27" xr3:uid="{94C00EC6-AB2D-4D90-B787-2C1FF57B5832}" name="MÊS" dataDxfId="182"/>
-    <tableColumn id="28" xr3:uid="{57AFB38B-E07E-457A-9571-EB539326E109}" name="SAFRA" dataDxfId="181"/>
-    <tableColumn id="29" xr3:uid="{FABF4B27-AD0C-443A-873A-01B8499E64E4}" name="TIPO" dataDxfId="180"/>
+    <tableColumn id="2" xr3:uid="{CD1BE27C-2122-4E57-BF75-B4E0FA407680}" name="ALGODÃO TOTAL" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{6AAC4787-45BB-49C3-925E-EB86773D0EE3}" name="ALGODÃO PLUMA" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{A709C33E-0EFD-439D-AFA6-DCBE5DFECC09}" name="ALGODÃO CAROÇO" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{36919ACC-6DBD-4BA6-B171-C06771CAA181}" name="AMENDOIM" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{A9E1ECF8-9280-4528-BB2D-F3444CC4E573}" name="ARROZ TOTAL" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{E24CCEF1-19C6-4E7E-8519-F2CBD6FFBD2C}" name="ARROZ SEQUEIRO" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{27262FD4-F510-4739-AE4D-503E89394540}" name="ARROZ IRRIGADO" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{07A828EE-65C2-453C-98A5-132A6F8EEB49}" name="FEIJÃO TOTAL" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{77436711-59D7-4D39-A13D-93314192FF57}" name="FEIJÃO CORES" dataDxfId="54"/>
+    <tableColumn id="11" xr3:uid="{C39CBBE1-C887-4FAA-B20D-BEF14F189268}" name="FEIJÃO PRETO" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{793D8F4C-ED63-45E7-81EC-8827A45470EF}" name="FEIJÃO CAUPI" dataDxfId="52"/>
+    <tableColumn id="13" xr3:uid="{59CC00D7-C96D-4832-9F17-68AA9395C332}" name="GERGELIM" dataDxfId="51"/>
+    <tableColumn id="14" xr3:uid="{6F397307-9E9A-4B49-89A4-0D105DC65A10}" name="GIRASSOL" dataDxfId="50"/>
+    <tableColumn id="15" xr3:uid="{76D545D2-CB23-48DD-AB8A-DAF6093C755D}" name="MAMONA" dataDxfId="49"/>
+    <tableColumn id="16" xr3:uid="{72E88D52-C6D2-4CF2-8498-8A5F1E83E6C7}" name="MILHO" dataDxfId="48"/>
+    <tableColumn id="17" xr3:uid="{4972AB7E-DAFC-42EA-8460-6CE3DFB48C04}" name="SOJA" dataDxfId="47"/>
+    <tableColumn id="18" xr3:uid="{C27C81AD-E84C-4DB4-9290-8E1075D91C93}" name="SORGO" dataDxfId="46"/>
+    <tableColumn id="19" xr3:uid="{0A447A82-E343-410A-8854-08B23C052F47}" name="AVEIA" dataDxfId="45"/>
+    <tableColumn id="20" xr3:uid="{F5ED3C8B-B7CB-452E-96A2-FCCEB899C54E}" name="CANOLA" dataDxfId="44"/>
+    <tableColumn id="21" xr3:uid="{17829594-1EEC-4783-9488-1309944A44E5}" name="CENTEIO" dataDxfId="43"/>
+    <tableColumn id="22" xr3:uid="{49B2C1E3-0396-4037-BB4B-32C18FDB6CC7}" name="CEVADA" dataDxfId="42"/>
+    <tableColumn id="23" xr3:uid="{C10C34AB-D106-4FB2-B097-C90EF653E9E5}" name="TRIGO" dataDxfId="41"/>
+    <tableColumn id="24" xr3:uid="{80045204-E6E2-42D6-9449-CCD3B9641988}" name="TRITICALE" dataDxfId="40"/>
+    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="39"/>
+    <tableColumn id="26" xr3:uid="{FA0650E0-02EE-433A-927B-8DCFAD627C43}" name="ANO" dataDxfId="38"/>
+    <tableColumn id="27" xr3:uid="{94C00EC6-AB2D-4D90-B787-2C1FF57B5832}" name="MÊS" dataDxfId="37"/>
+    <tableColumn id="28" xr3:uid="{57AFB38B-E07E-457A-9571-EB539326E109}" name="SAFRA" dataDxfId="36"/>
+    <tableColumn id="29" xr3:uid="{FABF4B27-AD0C-443A-873A-01B8499E64E4}" name="TIPO" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1448,7 +1448,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y38" sqref="Y38"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2:AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,13 +1597,13 @@
         <v>35</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -1618,58 +1618,58 @@
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>357.8</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>15.1</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
+        <v>312.60000000000002</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>1218.5</v>
       </c>
       <c r="U2" s="1">
-        <v>0</v>
+        <v>1161.8</v>
       </c>
       <c r="V2" s="1">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="W2" s="1">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <v>0</v>
+        <v>40.1</v>
       </c>
       <c r="Z2" s="1">
-        <v>0</v>
+        <v>27.2</v>
       </c>
       <c r="AA2" s="1">
         <v>0</v>
@@ -1678,13 +1678,13 @@
         <v>0</v>
       </c>
       <c r="AC2" s="1">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="AD2" s="1">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AE2" s="1">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AF2" s="1">
         <v>0</v>
@@ -1693,13 +1693,13 @@
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>0</v>
+        <v>373.3</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
+        <v>1260.1999999999998</v>
       </c>
       <c r="AJ2" s="1">
-        <v>0</v>
+        <v>1633.4999999999998</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>65</v>
@@ -1719,13 +1719,13 @@
         <v>36</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -1740,58 +1740,58 @@
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
+        <v>357.8</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>15.1</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R3" s="1">
         <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
+        <v>312.60000000000002</v>
       </c>
       <c r="T3" s="1">
-        <v>0</v>
+        <v>1218.5</v>
       </c>
       <c r="U3" s="1">
-        <v>0</v>
+        <v>1161.8</v>
       </c>
       <c r="V3" s="1">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="W3" s="1">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="X3" s="1">
         <v>0</v>
       </c>
       <c r="Y3" s="1">
-        <v>0</v>
+        <v>40.1</v>
       </c>
       <c r="Z3" s="1">
-        <v>0</v>
+        <v>27.2</v>
       </c>
       <c r="AA3" s="1">
         <v>0</v>
@@ -1800,13 +1800,13 @@
         <v>0</v>
       </c>
       <c r="AC3" s="1">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="AD3" s="1">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AE3" s="1">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AF3" s="1">
         <v>0</v>
@@ -1815,13 +1815,13 @@
         <v>0</v>
       </c>
       <c r="AH3" s="1">
-        <v>0</v>
+        <v>373.3</v>
       </c>
       <c r="AI3" s="1">
-        <v>0</v>
+        <v>1260.1999999999998</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0</v>
+        <v>1633.4999999999998</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>65</v>
@@ -1841,13 +1841,13 @@
         <v>37</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -1862,58 +1862,58 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>357.8</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>15.1</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>312.60000000000002</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>1218.5</v>
       </c>
       <c r="U4" s="1">
-        <v>0</v>
+        <v>1161.8</v>
       </c>
       <c r="V4" s="1">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="W4" s="1">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="X4" s="1">
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>0</v>
+        <v>40.1</v>
       </c>
       <c r="Z4" s="1">
-        <v>0</v>
+        <v>27.2</v>
       </c>
       <c r="AA4" s="1">
         <v>0</v>
@@ -1922,13 +1922,13 @@
         <v>0</v>
       </c>
       <c r="AC4" s="1">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="AD4" s="1">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AE4" s="1">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AF4" s="1">
         <v>0</v>
@@ -1937,13 +1937,13 @@
         <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <v>0</v>
+        <v>373.3</v>
       </c>
       <c r="AI4" s="1">
-        <v>0</v>
+        <v>1260.1999999999998</v>
       </c>
       <c r="AJ4" s="1">
-        <v>0</v>
+        <v>1633.4999999999998</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>65</v>
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -1996,13 +1996,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -2014,16 +2014,16 @@
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
       </c>
       <c r="V5" s="1">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="W5" s="1">
         <v>0</v>
@@ -2032,10 +2032,10 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>0</v>
+        <v>206.1</v>
       </c>
       <c r="Z5" s="1">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AA5" s="1">
         <v>0</v>
@@ -2044,28 +2044,28 @@
         <v>0</v>
       </c>
       <c r="AC5" s="1">
-        <v>0</v>
+        <v>193.6</v>
       </c>
       <c r="AD5" s="1">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="AE5" s="1">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="AF5" s="1">
         <v>0</v>
       </c>
       <c r="AG5" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AH5" s="1">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="AI5" s="1">
-        <v>0</v>
+        <v>216.8</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0</v>
+        <v>220.5</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>65</v>
@@ -2085,109 +2085,109 @@
         <v>38</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>175.4</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>33.4</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>34.1</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>87.7</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>154.29999999999998</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>94.6</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>44.6</v>
       </c>
       <c r="M6" s="1">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="O6" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="Q6" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="R6" s="1">
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="S6" s="1">
         <v>0</v>
       </c>
       <c r="T6" s="1">
-        <v>0</v>
+        <v>96.3</v>
       </c>
       <c r="U6" s="1">
-        <v>0</v>
+        <v>74.5</v>
       </c>
       <c r="V6" s="1">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="W6" s="1">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="X6" s="1">
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>0</v>
+        <v>11.3</v>
       </c>
       <c r="Z6" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA6" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB6" s="1">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AC6" s="1">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="AD6" s="1">
-        <v>0</v>
+        <v>1030.4000000000001</v>
       </c>
       <c r="AE6" s="1">
-        <v>0</v>
+        <v>20.900000000000002</v>
       </c>
       <c r="AF6" s="1">
-        <v>0</v>
+        <v>146.9</v>
       </c>
       <c r="AG6" s="1">
-        <v>0</v>
+        <v>862.6</v>
       </c>
       <c r="AH6" s="1">
-        <v>0</v>
+        <v>329.7</v>
       </c>
       <c r="AI6" s="1">
-        <v>0</v>
+        <v>1138</v>
       </c>
       <c r="AJ6" s="1">
-        <v>0</v>
+        <v>1467.7</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>65</v>
@@ -2207,46 +2207,46 @@
         <v>34</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>33.4</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>29.8</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>135.6</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>91.5</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>40.1</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
@@ -2261,10 +2261,10 @@
         <v>0</v>
       </c>
       <c r="T7" s="1">
-        <v>0</v>
+        <v>74.5</v>
       </c>
       <c r="U7" s="1">
-        <v>0</v>
+        <v>74.5</v>
       </c>
       <c r="V7" s="1">
         <v>0</v>
@@ -2276,25 +2276,25 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="Z7" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AA7" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB7" s="1">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AC7" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AD7" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AE7" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AF7" s="1">
         <v>0</v>
@@ -2303,13 +2303,13 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>0</v>
+        <v>212.5</v>
       </c>
       <c r="AI7" s="1">
-        <v>0</v>
+        <v>78.399999999999991</v>
       </c>
       <c r="AJ7" s="1">
-        <v>0</v>
+        <v>290.89999999999998</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>65</v>
@@ -2329,10 +2329,10 @@
         <v>39</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>98.5</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -2347,61 +2347,61 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>4.3</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>82.2</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
+        <v>18.7</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="L8" s="1">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="M8" s="1">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="N8" s="1">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="Q8" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="R8" s="1">
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
       </c>
       <c r="T8" s="1">
-        <v>0</v>
+        <v>21.8</v>
       </c>
       <c r="U8" s="1">
         <v>0</v>
       </c>
       <c r="V8" s="1">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="W8" s="1">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="X8" s="1">
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="Z8" s="1">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="AA8" s="1">
         <v>0</v>
@@ -2410,28 +2410,28 @@
         <v>0</v>
       </c>
       <c r="AC8" s="1">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="AD8" s="1">
-        <v>0</v>
+        <v>1028.5999999999999</v>
       </c>
       <c r="AE8" s="1">
-        <v>0</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="AF8" s="1">
-        <v>0</v>
+        <v>146.9</v>
       </c>
       <c r="AG8" s="1">
-        <v>0</v>
+        <v>862.6</v>
       </c>
       <c r="AH8" s="1">
-        <v>0</v>
+        <v>117.2</v>
       </c>
       <c r="AI8" s="1">
-        <v>0</v>
+        <v>1059.5999999999999</v>
       </c>
       <c r="AJ8" s="1">
-        <v>0</v>
+        <v>1176.8</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>65</v>
@@ -2451,109 +2451,109 @@
         <v>40</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>106.9</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>27.900000000000002</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <v>64.5</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>1448.2</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>50.4</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>192.79999999999998</v>
       </c>
       <c r="M9" s="1">
-        <v>0</v>
+        <v>361.8</v>
       </c>
       <c r="N9" s="1">
-        <v>0</v>
+        <v>52.3</v>
       </c>
       <c r="O9" s="1">
-        <v>0</v>
+        <v>103.5</v>
       </c>
       <c r="P9" s="1">
-        <v>0</v>
+        <v>224.5</v>
       </c>
       <c r="Q9" s="1">
-        <v>0</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="R9" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S9" s="1">
-        <v>0</v>
+        <v>432.1</v>
       </c>
       <c r="T9" s="1">
-        <v>0</v>
+        <v>270.7</v>
       </c>
       <c r="U9" s="1">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="V9" s="1">
-        <v>0</v>
+        <v>7.1000000000000005</v>
       </c>
       <c r="W9" s="1">
-        <v>0</v>
+        <v>106.4</v>
       </c>
       <c r="X9" s="1">
-        <v>0</v>
+        <v>14.2</v>
       </c>
       <c r="Y9" s="1">
-        <v>0</v>
+        <v>399.59999999999997</v>
       </c>
       <c r="Z9" s="1">
-        <v>0</v>
+        <v>318.29999999999995</v>
       </c>
       <c r="AA9" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="AB9" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC9" s="1">
-        <v>0</v>
+        <v>71.3</v>
       </c>
       <c r="AD9" s="1">
-        <v>0</v>
+        <v>533.19999999999993</v>
       </c>
       <c r="AE9" s="1">
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="AF9" s="1">
-        <v>0</v>
+        <v>59.4</v>
       </c>
       <c r="AG9" s="1">
-        <v>0</v>
+        <v>53.8</v>
       </c>
       <c r="AH9" s="1">
-        <v>0</v>
+        <v>1555.1000000000001</v>
       </c>
       <c r="AI9" s="1">
-        <v>0</v>
+        <v>1203.5</v>
       </c>
       <c r="AJ9" s="1">
-        <v>0</v>
+        <v>2758.6000000000004</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>65</v>
@@ -2573,13 +2573,13 @@
         <v>41</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -2588,16 +2588,16 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>4.3</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>369.29999999999995</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -2606,76 +2606,76 @@
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <v>0</v>
+        <v>26.7</v>
       </c>
       <c r="P10" s="1">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="1">
-        <v>0</v>
+        <v>24.4</v>
       </c>
       <c r="R10" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S10" s="1">
-        <v>0</v>
+        <v>229.5</v>
       </c>
       <c r="T10" s="1">
-        <v>0</v>
+        <v>194.9</v>
       </c>
       <c r="U10" s="1">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="V10" s="1">
-        <v>0</v>
+        <v>7.1000000000000005</v>
       </c>
       <c r="W10" s="1">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="X10" s="1">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="Y10" s="1">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="Z10" s="1">
-        <v>0</v>
+        <v>287.39999999999998</v>
       </c>
       <c r="AA10" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="AB10" s="1">
         <v>0</v>
       </c>
       <c r="AC10" s="1">
-        <v>0</v>
+        <v>71.3</v>
       </c>
       <c r="AD10" s="1">
-        <v>0</v>
+        <v>215.10000000000002</v>
       </c>
       <c r="AE10" s="1">
-        <v>0</v>
+        <v>188.10000000000002</v>
       </c>
       <c r="AF10" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AG10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH10" s="1">
-        <v>0</v>
+        <v>378.09999999999997</v>
       </c>
       <c r="AI10" s="1">
-        <v>0</v>
+        <v>777.80000000000007</v>
       </c>
       <c r="AJ10" s="1">
-        <v>0</v>
+        <v>1155.9000000000001</v>
       </c>
       <c r="AK10" s="2" t="s">
         <v>65</v>
@@ -2719,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>18.2</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
@@ -2734,10 +2734,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" s="1">
-        <v>0</v>
+        <v>16.2</v>
       </c>
       <c r="Q11" s="1">
         <v>0</v>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="U11" s="1">
         <v>0</v>
@@ -2761,43 +2761,43 @@
         <v>0</v>
       </c>
       <c r="X11" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="Y11" s="1">
-        <v>0</v>
+        <v>15.6</v>
       </c>
       <c r="Z11" s="1">
-        <v>0</v>
+        <v>14.7</v>
       </c>
       <c r="AA11" s="1">
         <v>0</v>
       </c>
       <c r="AB11" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC11" s="1">
         <v>0</v>
       </c>
       <c r="AD11" s="1">
-        <v>0</v>
+        <v>318.10000000000002</v>
       </c>
       <c r="AE11" s="1">
-        <v>0</v>
+        <v>231.9</v>
       </c>
       <c r="AF11" s="1">
-        <v>0</v>
+        <v>40.4</v>
       </c>
       <c r="AG11" s="1">
-        <v>0</v>
+        <v>45.8</v>
       </c>
       <c r="AH11" s="1">
-        <v>0</v>
+        <v>18.2</v>
       </c>
       <c r="AI11" s="1">
-        <v>0</v>
+        <v>334.90000000000003</v>
       </c>
       <c r="AJ11" s="1">
-        <v>0</v>
+        <v>353.1</v>
       </c>
       <c r="AK11" s="2" t="s">
         <v>65</v>
@@ -2817,79 +2817,79 @@
         <v>43</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>98.100000000000009</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>23.6</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>64.2</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
+        <v>1060.6999999999998</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>50.4</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>192.79999999999998</v>
       </c>
       <c r="M12" s="1">
-        <v>0</v>
+        <v>357.3</v>
       </c>
       <c r="N12" s="1">
-        <v>0</v>
+        <v>52.3</v>
       </c>
       <c r="O12" s="1">
-        <v>0</v>
+        <v>74.8</v>
       </c>
       <c r="P12" s="1">
-        <v>0</v>
+        <v>124.3</v>
       </c>
       <c r="Q12" s="1">
-        <v>0</v>
+        <v>6.2</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12" s="1">
-        <v>0</v>
+        <v>202.6</v>
       </c>
       <c r="T12" s="1">
-        <v>0</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="U12" s="1">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="V12" s="1">
         <v>0</v>
       </c>
       <c r="W12" s="1">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="X12" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Y12" s="1">
-        <v>0</v>
+        <v>16.200000000000003</v>
       </c>
       <c r="Z12" s="1">
-        <v>0</v>
+        <v>16.200000000000003</v>
       </c>
       <c r="AA12" s="1">
         <v>0</v>
@@ -2913,13 +2913,13 @@
         <v>0</v>
       </c>
       <c r="AH12" s="1">
-        <v>0</v>
+        <v>1158.7999999999997</v>
       </c>
       <c r="AI12" s="1">
-        <v>0</v>
+        <v>90.8</v>
       </c>
       <c r="AJ12" s="1">
-        <v>0</v>
+        <v>1249.5999999999997</v>
       </c>
       <c r="AK12" s="2" t="s">
         <v>65</v>
@@ -2939,7 +2939,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>108.1</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -2957,10 +2957,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <v>33.1</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
@@ -2993,16 +2993,16 @@
         <v>0</v>
       </c>
       <c r="T13" s="1">
-        <v>0</v>
+        <v>176.2</v>
       </c>
       <c r="U13" s="1">
-        <v>0</v>
+        <v>173.2</v>
       </c>
       <c r="V13" s="1">
         <v>0</v>
       </c>
       <c r="W13" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X13" s="1">
         <v>0</v>
@@ -3035,13 +3035,13 @@
         <v>0</v>
       </c>
       <c r="AH13" s="1">
-        <v>0</v>
+        <v>108.1</v>
       </c>
       <c r="AI13" s="1">
-        <v>0</v>
+        <v>176.2</v>
       </c>
       <c r="AJ13" s="1">
-        <v>0</v>
+        <v>284.29999999999995</v>
       </c>
       <c r="AK13" s="2" t="s">
         <v>65</v>
@@ -3115,25 +3115,25 @@
         <v>0</v>
       </c>
       <c r="T14" s="1">
-        <v>0</v>
+        <v>35.900000000000006</v>
       </c>
       <c r="U14" s="1">
-        <v>0</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="V14" s="1">
         <v>0</v>
       </c>
       <c r="W14" s="1">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="X14" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="Y14" s="1">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="Z14" s="1">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="AA14" s="1">
         <v>0</v>
@@ -3145,7 +3145,7 @@
         <v>0</v>
       </c>
       <c r="AD14" s="1">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="AE14" s="1">
         <v>0</v>
@@ -3154,16 +3154,16 @@
         <v>0</v>
       </c>
       <c r="AG14" s="1">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="AH14" s="1">
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <v>0</v>
+        <v>41.1</v>
       </c>
       <c r="AJ14" s="1">
-        <v>0</v>
+        <v>41.1</v>
       </c>
       <c r="AK14" s="2" t="s">
         <v>65</v>
@@ -3207,7 +3207,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>51.4</v>
       </c>
       <c r="K15" s="1">
         <v>0</v>
@@ -3216,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="1">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="N15" s="1">
         <v>0</v>
@@ -3234,13 +3234,13 @@
         <v>0</v>
       </c>
       <c r="S15" s="1">
-        <v>0</v>
+        <v>50.8</v>
       </c>
       <c r="T15" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="U15" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="V15" s="1">
         <v>0</v>
@@ -3279,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="AH15" s="1">
-        <v>0</v>
+        <v>51.4</v>
       </c>
       <c r="AI15" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AJ15" s="1">
-        <v>0</v>
+        <v>52.199999999999996</v>
       </c>
       <c r="AK15" s="2" t="s">
         <v>65</v>
@@ -3305,109 +3305,109 @@
         <v>47</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>1205.9000000000001</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>291.5</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>51.6</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>5.7</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>408.5</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>430.79999999999995</v>
       </c>
       <c r="J16" s="1">
-        <v>0</v>
+        <v>3278.1999999999994</v>
       </c>
       <c r="K16" s="1">
-        <v>0</v>
+        <v>608.5</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>587.79999999999995</v>
       </c>
       <c r="M16" s="1">
-        <v>0</v>
+        <v>588.29999999999995</v>
       </c>
       <c r="N16" s="1">
-        <v>0</v>
+        <v>51.1</v>
       </c>
       <c r="O16" s="1">
-        <v>0</v>
+        <v>119.5</v>
       </c>
       <c r="P16" s="1">
-        <v>0</v>
+        <v>247.2</v>
       </c>
       <c r="Q16" s="1">
-        <v>0</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="R16" s="1">
-        <v>0</v>
+        <v>182.2</v>
       </c>
       <c r="S16" s="1">
-        <v>0</v>
+        <v>853.40000000000009</v>
       </c>
       <c r="T16" s="1">
-        <v>0</v>
+        <v>11365.000000000002</v>
       </c>
       <c r="U16" s="1">
-        <v>0</v>
+        <v>7240</v>
       </c>
       <c r="V16" s="1">
-        <v>0</v>
+        <v>2201.7000000000003</v>
       </c>
       <c r="W16" s="1">
-        <v>0</v>
+        <v>1867.2</v>
       </c>
       <c r="X16" s="1">
-        <v>0</v>
+        <v>56.1</v>
       </c>
       <c r="Y16" s="1">
-        <v>0</v>
+        <v>2033.6</v>
       </c>
       <c r="Z16" s="1">
-        <v>0</v>
+        <v>1278.5</v>
       </c>
       <c r="AA16" s="1">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="AB16" s="1">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="AC16" s="1">
-        <v>0</v>
+        <v>740.09999999999991</v>
       </c>
       <c r="AD16" s="1">
-        <v>0</v>
+        <v>4090.2</v>
       </c>
       <c r="AE16" s="1">
-        <v>0</v>
+        <v>2910</v>
       </c>
       <c r="AF16" s="1">
-        <v>0</v>
+        <v>348.7</v>
       </c>
       <c r="AG16" s="1">
-        <v>0</v>
+        <v>831.5</v>
       </c>
       <c r="AH16" s="1">
-        <v>0</v>
+        <v>4484.0999999999995</v>
       </c>
       <c r="AI16" s="1">
-        <v>0</v>
+        <v>17488.800000000003</v>
       </c>
       <c r="AJ16" s="1">
-        <v>0</v>
+        <v>21972.9</v>
       </c>
       <c r="AK16" s="2" t="s">
         <v>65</v>
@@ -3427,40 +3427,40 @@
         <v>48</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>2850.9</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>497.1</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>11.4</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>6.9</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>939.5</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>1269.5</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>3962.6</v>
       </c>
       <c r="K17" s="1">
-        <v>0</v>
+        <v>1111.7</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>926.4</v>
       </c>
       <c r="M17" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="N17" s="1">
         <v>0</v>
@@ -3472,34 +3472,34 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
       </c>
       <c r="S17" s="1">
-        <v>0</v>
+        <v>1919.7</v>
       </c>
       <c r="T17" s="1">
-        <v>0</v>
+        <v>20217.199999999997</v>
       </c>
       <c r="U17" s="1">
-        <v>0</v>
+        <v>11819.4</v>
       </c>
       <c r="V17" s="1">
-        <v>0</v>
+        <v>3764.3</v>
       </c>
       <c r="W17" s="1">
-        <v>0</v>
+        <v>4547.3999999999996</v>
       </c>
       <c r="X17" s="1">
-        <v>0</v>
+        <v>86.1</v>
       </c>
       <c r="Y17" s="1">
-        <v>0</v>
+        <v>3435.1000000000004</v>
       </c>
       <c r="Z17" s="1">
-        <v>0</v>
+        <v>2167.3000000000002</v>
       </c>
       <c r="AA17" s="1">
         <v>0</v>
@@ -3508,28 +3508,28 @@
         <v>0</v>
       </c>
       <c r="AC17" s="1">
-        <v>0</v>
+        <v>1267.8</v>
       </c>
       <c r="AD17" s="1">
-        <v>0</v>
+        <v>13096.1</v>
       </c>
       <c r="AE17" s="1">
-        <v>0</v>
+        <v>5810.5</v>
       </c>
       <c r="AF17" s="1">
-        <v>0</v>
+        <v>730.5</v>
       </c>
       <c r="AG17" s="1">
-        <v>0</v>
+        <v>6555.1</v>
       </c>
       <c r="AH17" s="1">
-        <v>0</v>
+        <v>6813.5</v>
       </c>
       <c r="AI17" s="1">
-        <v>0</v>
+        <v>36748.399999999994</v>
       </c>
       <c r="AJ17" s="1">
-        <v>0</v>
+        <v>43561.899999999994</v>
       </c>
       <c r="AK17" s="2" t="s">
         <v>65</v>
@@ -3549,7 +3549,7 @@
         <v>49</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -3567,25 +3567,25 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>23.1</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>52.3</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>200.6</v>
       </c>
       <c r="K18" s="1">
-        <v>0</v>
+        <v>9.9</v>
       </c>
       <c r="L18" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M18" s="1">
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="O18" s="1">
         <v>0</v>
@@ -3600,28 +3600,28 @@
         <v>0</v>
       </c>
       <c r="S18" s="1">
-        <v>0</v>
+        <v>176.1</v>
       </c>
       <c r="T18" s="1">
-        <v>0</v>
+        <v>588.79999999999995</v>
       </c>
       <c r="U18" s="1">
-        <v>0</v>
+        <v>63.8</v>
       </c>
       <c r="V18" s="1">
-        <v>0</v>
+        <v>131.30000000000001</v>
       </c>
       <c r="W18" s="1">
-        <v>0</v>
+        <v>384.7</v>
       </c>
       <c r="X18" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Y18" s="1">
-        <v>0</v>
+        <v>342.2</v>
       </c>
       <c r="Z18" s="1">
-        <v>0</v>
+        <v>327.2</v>
       </c>
       <c r="AA18" s="1">
         <v>0</v>
@@ -3630,13 +3630,13 @@
         <v>0</v>
       </c>
       <c r="AC18" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD18" s="1">
-        <v>0</v>
+        <v>18.3</v>
       </c>
       <c r="AE18" s="1">
-        <v>0</v>
+        <v>18.3</v>
       </c>
       <c r="AF18" s="1">
         <v>0</v>
@@ -3645,13 +3645,13 @@
         <v>0</v>
       </c>
       <c r="AH18" s="1">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="AI18" s="1">
-        <v>0</v>
+        <v>949.3</v>
       </c>
       <c r="AJ18" s="1">
-        <v>0</v>
+        <v>1225.3</v>
       </c>
       <c r="AK18" s="2" t="s">
         <v>65</v>
@@ -3725,13 +3725,13 @@
         <v>0</v>
       </c>
       <c r="T19" s="1">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="U19" s="1">
         <v>0</v>
       </c>
       <c r="V19" s="1">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="W19" s="1">
         <v>0</v>
@@ -3755,25 +3755,25 @@
         <v>0</v>
       </c>
       <c r="AD19" s="1">
-        <v>0</v>
+        <v>448.7</v>
       </c>
       <c r="AE19" s="1">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="AF19" s="1">
         <v>0</v>
       </c>
       <c r="AG19" s="1">
-        <v>0</v>
+        <v>341.7</v>
       </c>
       <c r="AH19" s="1">
         <v>0</v>
       </c>
       <c r="AI19" s="1">
-        <v>0</v>
+        <v>497.7</v>
       </c>
       <c r="AJ19" s="1">
-        <v>0</v>
+        <v>497.7</v>
       </c>
       <c r="AK19" s="2" t="s">
         <v>65</v>
@@ -3877,25 +3877,25 @@
         <v>0</v>
       </c>
       <c r="AD20" s="1">
-        <v>0</v>
+        <v>55.199999999999996</v>
       </c>
       <c r="AE20" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AF20" s="1">
         <v>0</v>
       </c>
       <c r="AG20" s="1">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="AH20" s="1">
         <v>0</v>
       </c>
       <c r="AI20" s="1">
-        <v>0</v>
+        <v>55.199999999999996</v>
       </c>
       <c r="AJ20" s="1">
-        <v>0</v>
+        <v>55.199999999999996</v>
       </c>
       <c r="AK20" s="2" t="s">
         <v>65</v>
@@ -3999,25 +3999,25 @@
         <v>0</v>
       </c>
       <c r="AD21" s="1">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="AE21" s="1">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="AF21" s="1">
         <v>0</v>
       </c>
       <c r="AG21" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AH21" s="1">
         <v>0</v>
       </c>
       <c r="AI21" s="1">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="AJ21" s="1">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="AK21" s="2" t="s">
         <v>65</v>
@@ -4121,25 +4121,25 @@
         <v>0</v>
       </c>
       <c r="AD22" s="1">
-        <v>0</v>
+        <v>123.30000000000001</v>
       </c>
       <c r="AE22" s="1">
-        <v>0</v>
+        <v>83.2</v>
       </c>
       <c r="AF22" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AG22" s="1">
-        <v>0</v>
+        <v>39.4</v>
       </c>
       <c r="AH22" s="1">
         <v>0</v>
       </c>
       <c r="AI22" s="1">
-        <v>0</v>
+        <v>123.30000000000001</v>
       </c>
       <c r="AJ22" s="1">
-        <v>0</v>
+        <v>123.30000000000001</v>
       </c>
       <c r="AK22" s="2" t="s">
         <v>65</v>
@@ -4183,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K23" s="1">
         <v>0</v>
@@ -4210,28 +4210,28 @@
         <v>0</v>
       </c>
       <c r="S23" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>83.7</v>
       </c>
       <c r="U23" s="1">
         <v>0</v>
       </c>
       <c r="V23" s="1">
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="W23" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="X23" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="Y23" s="1">
-        <v>0</v>
+        <v>204.60000000000002</v>
       </c>
       <c r="Z23" s="1">
-        <v>0</v>
+        <v>108.9</v>
       </c>
       <c r="AA23" s="1">
         <v>0</v>
@@ -4240,28 +4240,28 @@
         <v>0</v>
       </c>
       <c r="AC23" s="1">
-        <v>0</v>
+        <v>95.7</v>
       </c>
       <c r="AD23" s="1">
-        <v>0</v>
+        <v>2790.8999999999996</v>
       </c>
       <c r="AE23" s="1">
-        <v>0</v>
+        <v>1195.8</v>
       </c>
       <c r="AF23" s="1">
-        <v>0</v>
+        <v>140.5</v>
       </c>
       <c r="AG23" s="1">
-        <v>0</v>
+        <v>1454.6</v>
       </c>
       <c r="AH23" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI23" s="1">
-        <v>0</v>
+        <v>3079.2</v>
       </c>
       <c r="AJ23" s="1">
-        <v>0</v>
+        <v>3086.2</v>
       </c>
       <c r="AK23" s="2" t="s">
         <v>65</v>
@@ -4350,7 +4350,7 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
@@ -4362,28 +4362,28 @@
         <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AD24" s="1">
-        <v>0</v>
+        <v>16.3</v>
       </c>
       <c r="AE24" s="1">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="AF24" s="1">
         <v>0</v>
       </c>
       <c r="AG24" s="1">
-        <v>0</v>
+        <v>5.8</v>
       </c>
       <c r="AH24" s="1">
         <v>0</v>
       </c>
       <c r="AI24" s="1">
-        <v>0</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="AJ24" s="1">
-        <v>0</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="AK24" s="2" t="s">
         <v>65</v>
@@ -4403,109 +4403,109 @@
         <v>56</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>4538.0999999999985</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>149.69999999999999</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>834</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>18.500000000000004</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>11.500000000000002</v>
       </c>
       <c r="H25" s="1">
-        <v>0</v>
+        <v>1508.1</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>1944.3000000000002</v>
       </c>
       <c r="J25" s="1">
-        <v>0</v>
+        <v>9463.7999999999993</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>1900.7</v>
       </c>
       <c r="L25" s="1">
-        <v>0</v>
+        <v>1780.6999999999996</v>
       </c>
       <c r="M25" s="1">
-        <v>0</v>
+        <v>961.09999999999991</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <v>105.1</v>
       </c>
       <c r="O25" s="1">
-        <v>0</v>
+        <v>225.7</v>
       </c>
       <c r="P25" s="1">
-        <v>0</v>
+        <v>471.9</v>
       </c>
       <c r="Q25" s="1">
-        <v>0</v>
+        <v>75.8</v>
       </c>
       <c r="R25" s="1">
-        <v>0</v>
+        <v>188.49999999999997</v>
       </c>
       <c r="S25" s="1">
-        <v>0</v>
+        <v>3754.2999999999997</v>
       </c>
       <c r="T25" s="1">
-        <v>0</v>
+        <v>34109.4</v>
       </c>
       <c r="U25" s="1">
-        <v>0</v>
+        <v>20684.699999999997</v>
       </c>
       <c r="V25" s="1">
-        <v>0</v>
+        <v>6217.6</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <v>7037.7999999999993</v>
       </c>
       <c r="X25" s="1">
-        <v>0</v>
+        <v>169.29999999999998</v>
       </c>
       <c r="Y25" s="1">
-        <v>0</v>
+        <v>6676.300000000002</v>
       </c>
       <c r="Z25" s="1">
-        <v>0</v>
+        <v>4244.8</v>
       </c>
       <c r="AA25" s="1">
-        <v>0</v>
+        <v>22.3</v>
       </c>
       <c r="AB25" s="1">
-        <v>0</v>
+        <v>3.0999999999999996</v>
       </c>
       <c r="AC25" s="1">
-        <v>0</v>
+        <v>2406.1000000000004</v>
       </c>
       <c r="AD25" s="1">
-        <v>0</v>
+        <v>22216.199999999997</v>
       </c>
       <c r="AE25" s="1">
-        <v>0</v>
+        <v>10584.299999999997</v>
       </c>
       <c r="AF25" s="1">
-        <v>0</v>
+        <v>1426.7000000000003</v>
       </c>
       <c r="AG25" s="1">
-        <v>0</v>
+        <v>10205.199999999999</v>
       </c>
       <c r="AH25" s="1">
-        <v>0</v>
+        <v>14001.9</v>
       </c>
       <c r="AI25" s="1">
-        <v>0</v>
+        <v>63001.899999999994</v>
       </c>
       <c r="AJ25" s="1">
-        <v>0</v>
+        <v>77003.8</v>
       </c>
       <c r="AK25" s="2" t="s">
         <v>65</v>
@@ -7664,7 +7664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A92389E-F363-478C-8FE0-DB1A38F4DB64}">
   <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B2" sqref="B2:AJ25"/>
     </sheetView>
@@ -17271,7 +17271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37856A1E-82E7-45AE-A2B0-C510B7D63887}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Y36" sqref="B2:Y36"/>
     </sheetView>

</xml_diff>